<commit_message>
Changed from is_deleted to status in company table
</commit_message>
<xml_diff>
--- a/CAAS_to_SYSDATA_mapping.xlsx
+++ b/CAAS_to_SYSDATA_mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="135">
   <si>
     <t>CAAS_ADMIN.ADV</t>
   </si>
@@ -393,15 +393,15 @@
     <t>username</t>
   </si>
   <si>
+    <t>where company_id =  (select id from company where company_type = 'Canoe') and location_type = 'Office'</t>
+  </si>
+  <si>
     <t>where phone_type = 'Main' and company_id  =  (select id from company where company_type = 'Canoe') and contact_id is null</t>
   </si>
   <si>
     <t>where phone_type = 'Fax' and company_id  =  (select id from company where company_type = 'Canoe') and contact_id is null</t>
   </si>
   <si>
-    <t>where company_id =  (select id from company where company_type = 'Canoe') and contact_id is null</t>
-  </si>
-  <si>
     <t>sysdata.phone.contact_id=sysdata.contact.id and sysdata.phone.type = 'Home'</t>
   </si>
   <si>
@@ -412,6 +412,15 @@
   </si>
   <si>
     <t>product_type_code</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Not in QA as of 16-FEB-2012</t>
+  </si>
+  <si>
+    <t>(case status when 'Active' then '1' else '0' end)</t>
   </si>
 </sst>
 </file>
@@ -808,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C126"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,1077 +830,1086 @@
     <col min="3" max="3" width="40.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>54</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>114</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>114</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>34</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>123</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>18</v>
+        <v>112</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>10</v>
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="4"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="4"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="4"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>18</v>
+        <v>66</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="4"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C85" s="3"/>
-    </row>
-    <row r="86" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="4"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="C88" s="3"/>
+    </row>
+    <row r="89" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>62</v>
+        <v>4</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B100" s="9">
-        <v>3</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>18</v>
+        <v>93</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="B103" s="9">
+        <v>3</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="4"/>
+      <c r="B107" s="5"/>
+      <c r="C107" s="4"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>62</v>
+        <v>4</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>114</v>
+        <v>99</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B117" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B118" s="11">
+      <c r="B121" s="11">
         <v>1</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+    <row r="122" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B122" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C122" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+    <row r="123" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B123" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C123" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+    <row r="124" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B124" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C124" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+    <row r="125" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B125" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="C125" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B126" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B127" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B128" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C128" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="126" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="4"/>
-      <c r="B126" s="5"/>
-      <c r="C126" s="4"/>
+    <row r="129" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="4"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>